<commit_message>
Ajout numéro TRE division territoriale cc41ddb4ef2e2fc474d8ef5205963d84f69089b4
</commit_message>
<xml_diff>
--- a/ig/majKereval/ValueSet-code-region-territorial-division.xlsx
+++ b/ig/majKereval/ValueSet-code-region-territorial-division.xlsx
@@ -61,7 +61,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2023-03-27T14:30:28+00:00</t>
+    <t>2023-03-27T14:49:55+00:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -97,16 +97,16 @@
     <t>https://mos.esante.gouv.fr/NOS/JDV_J230-CommuneOM-ROR/FHIR/JDV-J230-CommuneOM-ROR</t>
   </si>
   <si>
-    <t>https://mos.esante.gouv.fr/NOS/JDV_JXXX-DepartementOM-ROR/FHIR/JDV-JXXX-DepartementOM-ROR</t>
+    <t>https://mos.esante.gouv.fr/NOS/JDV_J248-DepartementOM-ROR/FHIR/JDV-J248-DepartementOM-ROR</t>
   </si>
   <si>
     <t>https://mos.esante.gouv.fr/NOS/JDV_J237-RegionOM-ROR/FHIR/JDV-J237-RegionOM-ROR</t>
   </si>
   <si>
-    <t>https://mos.esante.gouv.fr/NOS/JDV_JXXX-TerritoireSante-ROR/FHIR/JDV-JXXX-TerritoireSante-ROR</t>
-  </si>
-  <si>
-    <t>https://mos.esante.gouv.fr/NOS/JDV_JXXX-Pays-ROR/FHIR/JDV-JXXX-Pays-ROR</t>
+    <t>https://mos.esante.gouv.fr/NOS/JDV_J249-TerritoireSante-ROR/FHIR/JDV-J249-TerritoireSante-ROR</t>
+  </si>
+  <si>
+    <t>https://mos.esante.gouv.fr/NOS/JDV_J247-Pays-ROR/FHIR/JDV-J247-Pays-ROR</t>
   </si>
 </sst>
 </file>

</xml_diff>